<commit_message>
PODCAT-1679: Download submission template does't updated with the new field
</commit_message>
<xml_diff>
--- a/public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE9A20E7-BF8D-4864-A084-1730E6915D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{1DBD8EDA-8D16-48B6-ABF1-40CB9C71B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C08D2315-AE61-4997-8AFF-498D044F191A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="232">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Data Update Type</t>
+  </si>
+  <si>
+    <t>Resource Contact URL</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
   <si>
     <t>Dataset ID</t>
@@ -741,7 +747,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,8 +844,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,8 +876,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -897,12 +915,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1018,6 +1049,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1342,8 +1377,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1487,7 +1522,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="17" spans="1:3" ht="15.6">
+    <row r="17" spans="1:5" ht="16.5">
       <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
@@ -1495,19 +1530,25 @@
         <v>22</v>
       </c>
       <c r="C17" s="38"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="E17" s="47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="36"/>
       <c r="B18" s="11"/>
       <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18" s="48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:5">
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="C21" s="6"/>
     </row>
   </sheetData>
@@ -1588,28 +1629,28 @@
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1663,28 +1704,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="51.75" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1701,13 +1742,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1724,13 +1765,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1747,13 +1788,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1770,13 +1811,13 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1793,13 +1834,13 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1816,13 +1857,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1839,13 +1880,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1862,13 +1903,13 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1885,13 +1926,13 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1908,13 +1949,13 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1931,13 +1972,13 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1954,13 +1995,13 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1977,13 +2018,13 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2000,13 +2041,13 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2023,13 +2064,13 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2046,13 +2087,13 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2069,13 +2110,13 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2092,13 +2133,13 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2115,13 +2156,13 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2138,13 +2179,13 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2161,13 +2202,13 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2184,13 +2225,13 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2207,13 +2248,13 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2230,13 +2271,13 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2253,13 +2294,13 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2276,13 +2317,13 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2299,13 +2340,13 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2322,13 +2363,13 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2345,13 +2386,13 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2368,13 +2409,13 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2391,13 +2432,13 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2414,13 +2455,13 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2437,13 +2478,13 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G34" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2460,13 +2501,13 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2483,13 +2524,13 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2506,13 +2547,13 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2529,13 +2570,13 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F38" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2552,13 +2593,13 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F39" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2575,13 +2616,13 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F40" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2598,13 +2639,13 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F41" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G41" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2621,13 +2662,13 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G42" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2644,13 +2685,13 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G43" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2667,13 +2708,13 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F44" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G44" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2690,13 +2731,13 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F45" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G45" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2713,13 +2754,13 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G46" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2736,13 +2777,13 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F47" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G47" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2759,13 +2800,13 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F48" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G48" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2782,13 +2823,13 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F49" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G49" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2805,13 +2846,13 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G50" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2828,13 +2869,13 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F51" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G51" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2851,13 +2892,13 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G52" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2874,13 +2915,13 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F53" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G53" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2897,13 +2938,13 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F54" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G54" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2920,13 +2961,13 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F55" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G55" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2943,13 +2984,13 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F56" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G56" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2966,13 +3007,13 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F57" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G57" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2989,13 +3030,13 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F58" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G58" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3012,13 +3053,13 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F59" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G59" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3035,13 +3076,13 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F60" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G60" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3058,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F61" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G61" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3081,13 +3122,13 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F62" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G62" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3104,13 +3145,13 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F63" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G63" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3127,13 +3168,13 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F64" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G64" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3150,13 +3191,13 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F65" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G65" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3173,13 +3214,13 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F66" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G66" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3196,13 +3237,13 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F67" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G67" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3219,13 +3260,13 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F68" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G68" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3242,13 +3283,13 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F69" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G69" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3265,13 +3306,13 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F70" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G70" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3288,13 +3329,13 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F71" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G71" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3311,13 +3352,13 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F72" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G72" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3334,13 +3375,13 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F73" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G73" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3357,13 +3398,13 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F74" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G74" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3380,13 +3421,13 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F75" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G75" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3403,13 +3444,13 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F76" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G76" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3426,13 +3467,13 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F77" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G77" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3449,13 +3490,13 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F78" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G78" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3472,13 +3513,13 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F79" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G79" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3495,13 +3536,13 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F80" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G80" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3518,13 +3559,13 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F81" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G81" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3541,13 +3582,13 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F82" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G82" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3564,13 +3605,13 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F83" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G83" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3587,13 +3628,13 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F84" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G84" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4580,19 +4621,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="33" customFormat="1">
       <c r="A1" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4600,16 +4641,16 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="31" customFormat="1">
@@ -4617,16 +4658,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>126</v>
-      </c>
       <c r="E3" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="31" customFormat="1" ht="29.1">
@@ -4634,16 +4675,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="31" customFormat="1">
@@ -4651,10 +4692,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="31" customFormat="1">
@@ -4662,16 +4703,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="31" customFormat="1" ht="29.1">
@@ -4679,10 +4720,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D7"/>
     </row>
@@ -4691,110 +4732,110 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="31" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="31" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="31" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="31" customFormat="1">
       <c r="A12" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="31" customFormat="1">
       <c r="A13" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="31" customFormat="1" ht="43.5">
       <c r="A14" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A15" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="31" customFormat="1">
       <c r="A16" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="31" customFormat="1">
@@ -4802,10 +4843,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="31" customFormat="1">
@@ -4813,234 +4854,234 @@
         <v>18</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="31" customFormat="1">
       <c r="A19" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="31" customFormat="1">
       <c r="A20" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="31" customFormat="1">
       <c r="A21" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1">
       <c r="A22" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="31" customFormat="1" ht="43.5">
       <c r="A23" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A24" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A25" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A26" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D26" s="41"/>
     </row>
     <row r="27" spans="1:5" s="31" customFormat="1" ht="57.95">
       <c r="A27" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="31" customFormat="1">
       <c r="A28" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A29" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="31" customFormat="1">
       <c r="A30" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="31" customFormat="1">
       <c r="A31" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="31" customFormat="1">
       <c r="A32" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A33" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A34" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="31" customFormat="1">
       <c r="A35" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="31" customFormat="1" ht="57.95">
@@ -5048,16 +5089,16 @@
         <v>12</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="31" customFormat="1" ht="29.1">
@@ -5065,16 +5106,16 @@
         <v>12</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="29.1">
@@ -5082,10 +5123,10 @@
         <v>12</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D38" s="31"/>
     </row>
@@ -5094,10 +5135,10 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E39"/>
     </row>
@@ -5106,10 +5147,10 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E40"/>
     </row>
@@ -5118,10 +5159,10 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E41"/>
     </row>
@@ -5130,10 +5171,10 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E42"/>
     </row>
@@ -5142,108 +5183,108 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E43" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29.1">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E44"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D45" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E45" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E46" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="29.1">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E47"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E48" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E49" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -5283,7 +5324,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5297,10 +5338,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C2" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B2&amp;" "&amp;CHAR(10)</f>
@@ -5308,24 +5349,24 @@
 </v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C3" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
@@ -5333,24 +5374,24 @@
 </v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C4" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
@@ -5360,10 +5401,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C5" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
@@ -5373,10 +5414,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C6" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
@@ -5386,10 +5427,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C7" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B7&amp;" "&amp;CHAR(10)</f>
@@ -5399,10 +5440,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C8" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B8&amp;" "&amp;CHAR(10)</f>
@@ -5420,8 +5461,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23634515e2fd75be5bfad7623104c70a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="305374924f9daf7f55b4f039a6f85780" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d2768cdbde6492a0492d94561974b69">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8301a1e8c200ff5d9a28910b74393c39" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <xsd:element name="properties">
@@ -5444,6 +5505,8 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5511,6 +5574,16 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="24" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -5654,34 +5727,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F2AA8D1-2DD3-4347-BA28-17A66FDC41D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076BA1F7-10AD-4937-A794-3EFA2EB27755}"/>
 </file>
</xml_diff>

<commit_message>
PODCAT-1679: Download submission template does't updated with the new field (#501)
</commit_message>
<xml_diff>
--- a/public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE9A20E7-BF8D-4864-A084-1730E6915D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{1DBD8EDA-8D16-48B6-ABF1-40CB9C71B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C08D2315-AE61-4997-8AFF-498D044F191A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="232">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Data Update Type</t>
+  </si>
+  <si>
+    <t>Resource Contact URL</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
   <si>
     <t>Dataset ID</t>
@@ -741,7 +747,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,8 +844,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,8 +876,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -897,12 +915,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1018,6 +1049,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1342,8 +1377,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1487,7 +1522,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="17" spans="1:3" ht="15.6">
+    <row r="17" spans="1:5" ht="16.5">
       <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
@@ -1495,19 +1530,25 @@
         <v>22</v>
       </c>
       <c r="C17" s="38"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="E17" s="47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="36"/>
       <c r="B18" s="11"/>
       <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18" s="48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:5">
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="C21" s="6"/>
     </row>
   </sheetData>
@@ -1588,28 +1629,28 @@
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1663,28 +1704,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="51.75" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1701,13 +1742,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1724,13 +1765,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1747,13 +1788,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1770,13 +1811,13 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1793,13 +1834,13 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1816,13 +1857,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1839,13 +1880,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1862,13 +1903,13 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1885,13 +1926,13 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1908,13 +1949,13 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1931,13 +1972,13 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1954,13 +1995,13 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1977,13 +2018,13 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2000,13 +2041,13 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2023,13 +2064,13 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2046,13 +2087,13 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2069,13 +2110,13 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2092,13 +2133,13 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2115,13 +2156,13 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2138,13 +2179,13 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2161,13 +2202,13 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2184,13 +2225,13 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2207,13 +2248,13 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2230,13 +2271,13 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2253,13 +2294,13 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2276,13 +2317,13 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2299,13 +2340,13 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2322,13 +2363,13 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2345,13 +2386,13 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2368,13 +2409,13 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2391,13 +2432,13 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2414,13 +2455,13 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2437,13 +2478,13 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G34" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2460,13 +2501,13 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2483,13 +2524,13 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2506,13 +2547,13 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2529,13 +2570,13 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F38" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2552,13 +2593,13 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F39" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2575,13 +2616,13 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F40" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2598,13 +2639,13 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F41" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G41" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2621,13 +2662,13 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G42" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2644,13 +2685,13 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G43" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2667,13 +2708,13 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F44" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G44" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2690,13 +2731,13 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F45" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G45" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2713,13 +2754,13 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G46" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2736,13 +2777,13 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F47" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G47" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2759,13 +2800,13 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F48" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G48" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2782,13 +2823,13 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F49" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G49" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2805,13 +2846,13 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G50" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2828,13 +2869,13 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F51" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G51" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2851,13 +2892,13 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G52" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2874,13 +2915,13 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F53" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G53" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2897,13 +2938,13 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F54" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G54" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2920,13 +2961,13 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F55" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G55" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2943,13 +2984,13 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F56" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G56" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2966,13 +3007,13 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F57" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G57" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2989,13 +3030,13 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F58" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G58" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3012,13 +3053,13 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F59" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G59" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3035,13 +3076,13 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F60" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G60" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3058,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F61" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G61" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3081,13 +3122,13 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F62" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G62" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3104,13 +3145,13 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F63" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G63" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3127,13 +3168,13 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F64" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G64" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3150,13 +3191,13 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F65" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G65" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3173,13 +3214,13 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F66" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G66" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3196,13 +3237,13 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F67" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G67" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3219,13 +3260,13 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F68" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G68" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3242,13 +3283,13 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F69" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G69" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3265,13 +3306,13 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F70" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G70" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3288,13 +3329,13 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F71" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G71" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3311,13 +3352,13 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F72" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G72" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3334,13 +3375,13 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F73" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G73" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3357,13 +3398,13 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F74" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G74" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3380,13 +3421,13 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F75" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G75" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3403,13 +3444,13 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F76" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G76" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3426,13 +3467,13 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F77" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G77" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3449,13 +3490,13 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F78" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G78" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3472,13 +3513,13 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F79" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G79" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3495,13 +3536,13 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F80" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G80" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3518,13 +3559,13 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F81" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G81" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3541,13 +3582,13 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F82" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G82" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3564,13 +3605,13 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F83" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G83" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3587,13 +3628,13 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F84" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G84" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4580,19 +4621,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="33" customFormat="1">
       <c r="A1" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4600,16 +4641,16 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="31" customFormat="1">
@@ -4617,16 +4658,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>126</v>
-      </c>
       <c r="E3" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="31" customFormat="1" ht="29.1">
@@ -4634,16 +4675,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="31" customFormat="1">
@@ -4651,10 +4692,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="31" customFormat="1">
@@ -4662,16 +4703,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="31" customFormat="1" ht="29.1">
@@ -4679,10 +4720,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D7"/>
     </row>
@@ -4691,110 +4732,110 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="31" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="31" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="31" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="31" customFormat="1">
       <c r="A12" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="31" customFormat="1">
       <c r="A13" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="31" customFormat="1" ht="43.5">
       <c r="A14" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A15" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="31" customFormat="1">
       <c r="A16" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="31" customFormat="1">
@@ -4802,10 +4843,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="31" customFormat="1">
@@ -4813,234 +4854,234 @@
         <v>18</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="31" customFormat="1">
       <c r="A19" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="31" customFormat="1">
       <c r="A20" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="31" customFormat="1">
       <c r="A21" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1">
       <c r="A22" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="31" customFormat="1" ht="43.5">
       <c r="A23" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A24" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A25" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A26" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D26" s="41"/>
     </row>
     <row r="27" spans="1:5" s="31" customFormat="1" ht="57.95">
       <c r="A27" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="31" customFormat="1">
       <c r="A28" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A29" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="31" customFormat="1">
       <c r="A30" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="31" customFormat="1">
       <c r="A31" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="31" customFormat="1">
       <c r="A32" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A33" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A34" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="31" customFormat="1">
       <c r="A35" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="31" customFormat="1" ht="57.95">
@@ -5048,16 +5089,16 @@
         <v>12</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="31" customFormat="1" ht="29.1">
@@ -5065,16 +5106,16 @@
         <v>12</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="29.1">
@@ -5082,10 +5123,10 @@
         <v>12</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D38" s="31"/>
     </row>
@@ -5094,10 +5135,10 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E39"/>
     </row>
@@ -5106,10 +5147,10 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E40"/>
     </row>
@@ -5118,10 +5159,10 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E41"/>
     </row>
@@ -5130,10 +5171,10 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E42"/>
     </row>
@@ -5142,108 +5183,108 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E43" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29.1">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E44"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D45" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E45" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E46" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="29.1">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E47"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E48" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E49" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -5283,7 +5324,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5297,10 +5338,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C2" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B2&amp;" "&amp;CHAR(10)</f>
@@ -5308,24 +5349,24 @@
 </v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C3" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
@@ -5333,24 +5374,24 @@
 </v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C4" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
@@ -5360,10 +5401,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C5" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
@@ -5373,10 +5414,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C6" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
@@ -5386,10 +5427,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C7" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B7&amp;" "&amp;CHAR(10)</f>
@@ -5399,10 +5440,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C8" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B8&amp;" "&amp;CHAR(10)</f>
@@ -5420,8 +5461,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23634515e2fd75be5bfad7623104c70a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="305374924f9daf7f55b4f039a6f85780" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d2768cdbde6492a0492d94561974b69">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8301a1e8c200ff5d9a28910b74393c39" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <xsd:element name="properties">
@@ -5444,6 +5505,8 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5511,6 +5574,16 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="24" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -5654,34 +5727,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F2AA8D1-2DD3-4347-BA28-17A66FDC41D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076BA1F7-10AD-4937-A794-3EFA2EB27755}"/>
 </file>
</xml_diff>